<commit_message>
update profile intros spreadsheet
</commit_message>
<xml_diff>
--- a/input/mapping/BFDR_Profile_Intros.xlsx
+++ b/input/mapping/BFDR_Profile_Intros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptran\Documents\vital_records_sandbox_ig-1\input\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E54324-1C8B-449A-BB76-53C6045BB78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF13256-622F-4BD1-86BD-CC7EA587D5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
   </bookViews>
@@ -1437,7 +1437,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1447,6 +1447,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1463,7 +1469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1487,6 +1493,11 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1805,9 +1816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F4FF00-73BE-417A-ACC1-ED7CA7395274}">
   <dimension ref="A1:H141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C144" sqref="C144"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2015,55 +2026,55 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+    <row r="10" spans="1:8" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="F10" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="F11" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="14" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generate vrcl content separately
</commit_message>
<xml_diff>
--- a/input/mapping/BFDR_Profile_Intros.xlsx
+++ b/input/mapping/BFDR_Profile_Intros.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptran\Documents\vital_records_sandbox_ig-1\input\mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptran\Documents\vital_records_sandbox_ig-2\input\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80D200F-9F28-4606-A4E0-CDAD04888994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2DBA75-FBC0-4150-8BFA-6CA5A91BC7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
   </bookViews>
   <sheets>
     <sheet name="BFDR" sheetId="1" r:id="rId1"/>
     <sheet name="VRDR" sheetId="2" r:id="rId2"/>
+    <sheet name="VRCL" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BFDR!$A$1:$H$141</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">VRCL!$A$1:$H$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="420">
   <si>
     <t>Bundle-document-bfdr</t>
   </si>
@@ -1408,6 +1410,54 @@
   </si>
   <si>
     <t>Observation-coded-initiating-fetal-death-cause-or-condition</t>
+  </si>
+  <si>
+    <t>ObservationEducationLevelVitalRecords</t>
+  </si>
+  <si>
+    <t>ExtensionPartialDateAbsentReasonVitalRecords</t>
+  </si>
+  <si>
+    <t>ExtensionBypassEditFlagVitalRecords</t>
+  </si>
+  <si>
+    <t>ExtensionCityCodeVitalRecords</t>
+  </si>
+  <si>
+    <t>ExtensionDistrictCodeVitalRecords</t>
+  </si>
+  <si>
+    <t>ExtensionPostDirectionalVitalRecords</t>
+  </si>
+  <si>
+    <t>ExtensionPreDirectionalVitalRecords</t>
+  </si>
+  <si>
+    <t>ExtensionStreetDesignatorVitalRecords</t>
+  </si>
+  <si>
+    <t>Extension-partial-date-absent-reason-vr</t>
+  </si>
+  <si>
+    <t>Extension-bypass-edit-flag-vr</t>
+  </si>
+  <si>
+    <t>Extension-city-code-vr</t>
+  </si>
+  <si>
+    <t>Extension-district-code-vr</t>
+  </si>
+  <si>
+    <t>Extension-post-directional-vr</t>
+  </si>
+  <si>
+    <t>Extension-pre-directional-vr</t>
+  </si>
+  <si>
+    <t>Extension-street-designator-vr</t>
+  </si>
+  <si>
+    <t>Observation-education-level-vr</t>
   </si>
 </sst>
 </file>
@@ -1816,9 +1866,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F4FF00-73BE-417A-ACC1-ED7CA7395274}">
   <dimension ref="A1:H141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D146" sqref="D146"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E130" sqref="D130:E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4854,7 +4904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7A17BA-FE82-4288-B686-95D9BC7A8AC0}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="B35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E38" sqref="E38:G38"/>
     </sheetView>
   </sheetViews>
@@ -5767,4 +5817,600 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9C431E-1590-45F1-9F5F-911CCFABB960}">
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="7"/>
+    <col min="2" max="2" width="42.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="76.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="55.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="154" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>29</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H28" xr:uid="{82F4FF00-73BE-417A-ACC1-ED7CA7395274}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H28">
+      <sortCondition ref="A1:A28"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove line break in spreadsheet
</commit_message>
<xml_diff>
--- a/input/mapping/BFDR_Profile_Intros.xlsx
+++ b/input/mapping/BFDR_Profile_Intros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpassas/Documents/current_projects/NVSS/vital_records_sandbox_ig/input/mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptran\Documents\vital_records_sandbox_ig-1\input\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABE1DDC-1B05-8D44-9F49-FF264C8BDF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E50BF60-5178-477E-8BDD-B6AA83D8826D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38720" yWindow="4920" windowWidth="29040" windowHeight="15740" activeTab="2" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
   </bookViews>
   <sheets>
     <sheet name="BFDR" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="VRCL" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BFDR!$A$1:$H$141</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BFDR!$A$1:$H$139</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">VRCL!$A$1:$H$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1852,27 +1852,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F4FF00-73BE-417A-ACC1-ED7CA7395274}">
-  <dimension ref="A1:H141"/>
+  <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A100" sqref="A100:XFD100"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C132" sqref="A132:XFD132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="7"/>
-    <col min="2" max="2" width="42.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="76.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="55.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="7"/>
+    <col min="2" max="2" width="42.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="76.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="55.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="154" style="3" customWidth="1"/>
     <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="7" max="7" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>194</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="270" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>54</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>60</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>64</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>65</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>70</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>71</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>72</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>73</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>74</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>75</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>76</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>77</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>78</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>79</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>80</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>81</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>82</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>83</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>84</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>85</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>86</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>87</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>88</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>89</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <v>90</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>91</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
         <v>93</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>94</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>95</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>96</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>97</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>98</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>99</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>100</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <v>101</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>102</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <v>103</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <v>104</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <v>105</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>106</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
         <v>108</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
         <v>109</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
         <v>110</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
         <v>111</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
         <v>112</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <v>113</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
         <v>114</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
         <v>115</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
         <v>116</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="7">
         <v>117</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="7">
         <v>118</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
         <v>119</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="7">
         <v>120</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
         <v>121</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
         <v>122</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="7">
         <v>123</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="7">
         <v>124</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="7">
         <v>125</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="7">
         <v>126</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="7">
         <v>127</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="7">
         <v>128</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="7">
         <v>129</v>
       </c>
@@ -4659,7 +4659,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="7">
         <v>130</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="7">
         <v>131</v>
       </c>
@@ -4699,166 +4699,166 @@
         <v>85</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="7">
+        <v>133</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H132" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="7">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="H133" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="7">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>173</v>
+        <v>359</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>84</v>
+        <v>329</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>104</v>
+        <v>255</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="7">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>359</v>
+        <v>109</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>329</v>
+        <v>1</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="7">
+        <v>137</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="7">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>196</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>109</v>
+        <v>362</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>86</v>
+        <v>363</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="H137" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="7">
-        <v>137</v>
-      </c>
-      <c r="B138" s="2" t="s">
+    <row r="138" spans="1:8" s="5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A138" s="11">
+        <v>139</v>
+      </c>
+      <c r="B138" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="C138" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>364</v>
+      <c r="C138" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="E138" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H138" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H138" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="7">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="G139" s="2" t="s">
-        <v>97</v>
+        <v>198</v>
       </c>
       <c r="H139" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="140" spans="1:8" s="5" customFormat="1" ht="144" x14ac:dyDescent="0.2">
-      <c r="A140" s="11">
-        <v>139</v>
-      </c>
-      <c r="B140" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C140" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D140" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="E140" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G140" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H140" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="7">
-        <v>140</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H141" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H142">
-    <sortCondition ref="A2:A142"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H140">
+    <sortCondition ref="A2:A140"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4874,18 +4874,18 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="51.5" customWidth="1"/>
-    <col min="5" max="5" width="110.6640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="30.5" customWidth="1"/>
-    <col min="7" max="7" width="27.5" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" customWidth="1"/>
+    <col min="5" max="5" width="110.7109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>194</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="350" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="225" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="320" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="300" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5789,25 +5789,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9C431E-1590-45F1-9F5F-911CCFABB960}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="7"/>
-    <col min="2" max="2" width="42.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="76.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="55.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="7"/>
+    <col min="2" max="2" width="42.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="76.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="55.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="154" style="3" customWidth="1"/>
     <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="7" max="7" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>194</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -5850,7 +5850,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -5890,7 +5890,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -5964,7 +5964,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>16</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>17</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>18</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>19</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>21</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>22</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>23</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>24</v>
       </c>
@@ -6230,7 +6230,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>25</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>26</v>
       </c>
@@ -6267,7 +6267,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>27</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>28</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>29</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>30</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>31</v>
       </c>

</xml_diff>